<commit_message>
modified the page a little bit
</commit_message>
<xml_diff>
--- a/Server/participants.xlsx
+++ b/Server/participants.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A73FBB-745D-42DA-9E5C-688A386F3A4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="תגובות לטופס 1" sheetId="1" r:id="rId4"/>
+    <sheet name="תגובות לטופס 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>חותמת זמן</t>
   </si>
@@ -49,26 +58,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -77,41 +87,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -301,26 +315,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="11" width="18.88"/>
+    <col min="1" max="11" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -337,35 +354,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>45269.99554878472</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>45269.99655069444</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A few more changes
</commit_message>
<xml_diff>
--- a/Server/participants.xlsx
+++ b/Server/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B18B4B0-03ED-47B7-A07A-8ABDAC452A82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3CC4C1-0754-47D5-82C0-9F2A7CFF0DE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>חותמת זמן</t>
   </si>
@@ -28,55 +28,52 @@
     <t>איך קוראים לך?</t>
   </si>
   <si>
-    <t>רון</t>
+    <t>שחקן א</t>
   </si>
   <si>
-    <t>אור</t>
+    <t>שחקן ב</t>
   </si>
   <si>
-    <t>אלכס</t>
+    <t>שחקן ג</t>
   </si>
   <si>
-    <t>היייי</t>
+    <t>שחקן ד</t>
   </si>
   <si>
-    <t>נועם</t>
+    <t>שחקן ה</t>
   </si>
   <si>
-    <t>עמרי</t>
+    <t>שחקן ו</t>
   </si>
   <si>
-    <t>איי</t>
+    <t>שחקן ז</t>
   </si>
   <si>
-    <t>שרי</t>
+    <t>שחקן ח</t>
   </si>
   <si>
-    <t>הקשבי</t>
+    <t>שחקן ט</t>
   </si>
   <si>
-    <t>המפקד</t>
+    <t>שחקן יא</t>
   </si>
   <si>
-    <t>דור</t>
+    <t>שחקן יב</t>
   </si>
   <si>
-    <t>גור</t>
+    <t>שחקן יג</t>
   </si>
   <si>
-    <t>אריה</t>
+    <t>שחקן יד</t>
   </si>
   <si>
-    <t>טון</t>
+    <t>שחקן טו</t>
   </si>
   <si>
-    <t>לא נתמך עי גוגל</t>
+    <t>שחקן טז</t>
   </si>
   <si>
-    <t>נכון</t>
-  </si>
-  <si>
-    <t>עוד אחד</t>
+    <t>שחקן יז</t>
   </si>
 </sst>
 </file>
@@ -365,8 +362,8 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -394,7 +391,9 @@
     <row r="2" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -407,7 +406,9 @@
     <row r="3" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -420,7 +421,9 @@
     <row r="4" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -433,7 +436,9 @@
     <row r="5" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -446,7 +451,9 @@
     <row r="6" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -459,7 +466,9 @@
     <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -472,7 +481,9 @@
     <row r="8" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -485,7 +496,9 @@
     <row r="9" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -498,7 +511,9 @@
     <row r="10" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -511,7 +526,9 @@
     <row r="11" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -524,7 +541,9 @@
     <row r="12" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -537,7 +556,9 @@
     <row r="13" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -550,7 +571,9 @@
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -561,12 +584,10 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>45284.782326388886</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -578,12 +599,10 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>45284.782384259262</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -595,12 +614,10 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>45284.782453703701</v>
-      </c>
+      <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -612,13 +629,9 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>45284.782569444447</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -629,13 +642,9 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>45284.782754629632</v>
-      </c>
+      <c r="A19" s="2"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -646,13 +655,9 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>45284.782812500001</v>
-      </c>
+      <c r="A20" s="2"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -663,13 +668,9 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>45284.782997685186</v>
-      </c>
+      <c r="A21" s="2"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C21" s="3"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -680,13 +681,9 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>45284.783055555556</v>
-      </c>
+      <c r="A22" s="2"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -697,13 +694,9 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>45284.783113425925</v>
-      </c>
+      <c r="A23" s="2"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -714,13 +707,9 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>45284.783194444448</v>
-      </c>
+      <c r="A24" s="2"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="3"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -731,13 +720,9 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>45284.783356481479</v>
-      </c>
+      <c r="A25" s="2"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="3"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -748,13 +733,9 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>45284.783414351848</v>
-      </c>
+      <c r="A26" s="2"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -765,13 +746,9 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>45284.783472222225</v>
-      </c>
+      <c r="A27" s="2"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="C27" s="3"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -782,13 +759,9 @@
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>45284.78361111111</v>
-      </c>
+      <c r="A28" s="2"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="C28" s="3"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -799,13 +772,9 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>45284.783715277779</v>
-      </c>
+      <c r="A29" s="2"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C29" s="3"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -816,13 +785,9 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>45284.783773148149</v>
-      </c>
+      <c r="A30" s="2"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -833,13 +798,9 @@
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>45284.783912037034</v>
-      </c>
+      <c r="A31" s="2"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>

</xml_diff>

<commit_message>
Some un-noticed changes, don't notice
</commit_message>
<xml_diff>
--- a/Server/participants.xlsx
+++ b/Server/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0F49D8-7337-47B9-B329-3C3BBCABBD65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57611E13-FC75-44D3-9E80-F58149ABC327}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>חותמת זמן</t>
   </si>
@@ -34,10 +34,7 @@
     <t>שחקן ב</t>
   </si>
   <si>
-    <t>שחקן ג</t>
-  </si>
-  <si>
-    <t>שחקן ד</t>
+    <t>Sahkan</t>
   </si>
   <si>
     <t>שחקן ה</t>
@@ -55,6 +52,9 @@
     <t>שחקן ט</t>
   </si>
   <si>
+    <t>שחקן י</t>
+  </si>
+  <si>
     <t>שחקן יא</t>
   </si>
   <si>
@@ -80,6 +80,99 @@
   </si>
   <si>
     <t>שחקן יט</t>
+  </si>
+  <si>
+    <t>שחקן כ</t>
+  </si>
+  <si>
+    <t>שחקן כא</t>
+  </si>
+  <si>
+    <t>שחקן כב</t>
+  </si>
+  <si>
+    <t>שחקן כג</t>
+  </si>
+  <si>
+    <t>שחקן כד</t>
+  </si>
+  <si>
+    <t>שחקן כה</t>
+  </si>
+  <si>
+    <t>שחקן כו</t>
+  </si>
+  <si>
+    <t>שחקן כז</t>
+  </si>
+  <si>
+    <t>שחקן כח</t>
+  </si>
+  <si>
+    <t>שחקן כט</t>
+  </si>
+  <si>
+    <t>שחקן ל</t>
+  </si>
+  <si>
+    <t>שחקן לא</t>
+  </si>
+  <si>
+    <t>שחקן לב</t>
+  </si>
+  <si>
+    <t>שחקן לג</t>
+  </si>
+  <si>
+    <t>שחקן לד</t>
+  </si>
+  <si>
+    <t>שחקן לה</t>
+  </si>
+  <si>
+    <t>שחקן לו</t>
+  </si>
+  <si>
+    <t>שחקן לז</t>
+  </si>
+  <si>
+    <t>שחקן לח</t>
+  </si>
+  <si>
+    <t>שחקן לט</t>
+  </si>
+  <si>
+    <t>שחקן מ</t>
+  </si>
+  <si>
+    <t>שחקן מא</t>
+  </si>
+  <si>
+    <t>שחקן מב</t>
+  </si>
+  <si>
+    <t>שחקן מג</t>
+  </si>
+  <si>
+    <t>שחקן מד</t>
+  </si>
+  <si>
+    <t>שחקן מה</t>
+  </si>
+  <si>
+    <t>שחקן מו</t>
+  </si>
+  <si>
+    <t>שחקן מז</t>
+  </si>
+  <si>
+    <t>שחקן מח</t>
+  </si>
+  <si>
+    <t>שחקן מט</t>
+  </si>
+  <si>
+    <t>שחקן נ</t>
   </si>
 </sst>
 </file>
@@ -368,8 +461,8 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -427,7 +520,7 @@
     <row r="4" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="1"/>
@@ -667,7 +760,9 @@
     <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -680,7 +775,9 @@
     <row r="21" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -693,7 +790,9 @@
     <row r="22" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -706,7 +805,9 @@
     <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -719,7 +820,9 @@
     <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -732,7 +835,9 @@
     <row r="25" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -745,7 +850,9 @@
     <row r="26" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -758,7 +865,9 @@
     <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -771,7 +880,9 @@
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -784,7 +895,9 @@
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -797,7 +910,9 @@
     <row r="30" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -810,7 +925,9 @@
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -823,7 +940,9 @@
     <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="C32" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -836,7 +955,9 @@
     <row r="33" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="C33" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -849,7 +970,9 @@
     <row r="34" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -862,7 +985,9 @@
     <row r="35" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -875,7 +1000,9 @@
     <row r="36" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -888,7 +1015,9 @@
     <row r="37" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -901,7 +1030,9 @@
     <row r="38" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -914,7 +1045,9 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="C39" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -927,7 +1060,9 @@
     <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="C40" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -940,7 +1075,9 @@
     <row r="41" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="C41" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -953,7 +1090,9 @@
     <row r="42" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -966,7 +1105,9 @@
     <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="C43" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -979,7 +1120,9 @@
     <row r="44" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -992,7 +1135,9 @@
     <row r="45" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="C45" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -1005,7 +1150,9 @@
     <row r="46" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="C46" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1018,7 +1165,9 @@
     <row r="47" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="C47" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -1031,7 +1180,9 @@
     <row r="48" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="C48" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -1044,7 +1195,9 @@
     <row r="49" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="C49" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -1057,7 +1210,9 @@
     <row r="50" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="C50" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2122,5 +2277,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some more server changes
</commit_message>
<xml_diff>
--- a/Server/participants.xlsx
+++ b/Server/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57611E13-FC75-44D3-9E80-F58149ABC327}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08561D4D-7A02-442C-AFBF-D4B0A024715E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>חותמת זמן</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>שחקן נ</t>
+  </si>
+  <si>
+    <t>שחקן נא</t>
+  </si>
+  <si>
+    <t>שחקן נב</t>
   </si>
 </sst>
 </file>
@@ -461,8 +467,8 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1231,9 @@
     <row r="51" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -1238,7 +1246,9 @@
     <row r="52" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>

</xml_diff>

<commit_message>
A Change in the Tournament Process
</commit_message>
<xml_diff>
--- a/Server/participants.xlsx
+++ b/Server/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\PycharmProjects\ShabatMadat\Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08561D4D-7A02-442C-AFBF-D4B0A024715E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB4B121-6646-4989-B071-00084241F85E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>חותמת זמן</t>
   </si>
@@ -28,157 +28,199 @@
     <t>איך קוראים לך?</t>
   </si>
   <si>
-    <t>שחקן א</t>
-  </si>
-  <si>
-    <t>שחקן ב</t>
-  </si>
-  <si>
-    <t>Sahkan</t>
-  </si>
-  <si>
-    <t>שחקן ה</t>
-  </si>
-  <si>
-    <t>שחקן ו</t>
-  </si>
-  <si>
-    <t>שחקן ז</t>
-  </si>
-  <si>
-    <t>שחקן ח</t>
-  </si>
-  <si>
-    <t>שחקן ט</t>
-  </si>
-  <si>
-    <t>שחקן י</t>
-  </si>
-  <si>
-    <t>שחקן יא</t>
-  </si>
-  <si>
-    <t>שחקן יב</t>
-  </si>
-  <si>
-    <t>שחקן יג</t>
-  </si>
-  <si>
-    <t>שחקן יד</t>
-  </si>
-  <si>
-    <t>שחקן טו</t>
-  </si>
-  <si>
-    <t>שחקן טז</t>
-  </si>
-  <si>
-    <t>שחקן יז</t>
-  </si>
-  <si>
-    <t>שחקן יח</t>
-  </si>
-  <si>
-    <t>שחקן יט</t>
-  </si>
-  <si>
-    <t>שחקן כ</t>
-  </si>
-  <si>
-    <t>שחקן כא</t>
-  </si>
-  <si>
-    <t>שחקן כב</t>
-  </si>
-  <si>
-    <t>שחקן כג</t>
-  </si>
-  <si>
-    <t>שחקן כד</t>
-  </si>
-  <si>
-    <t>שחקן כה</t>
-  </si>
-  <si>
-    <t>שחקן כו</t>
-  </si>
-  <si>
-    <t>שחקן כז</t>
-  </si>
-  <si>
-    <t>שחקן כח</t>
-  </si>
-  <si>
-    <t>שחקן כט</t>
-  </si>
-  <si>
-    <t>שחקן ל</t>
-  </si>
-  <si>
-    <t>שחקן לא</t>
-  </si>
-  <si>
-    <t>שחקן לב</t>
-  </si>
-  <si>
-    <t>שחקן לג</t>
-  </si>
-  <si>
-    <t>שחקן לד</t>
-  </si>
-  <si>
-    <t>שחקן לה</t>
-  </si>
-  <si>
-    <t>שחקן לו</t>
-  </si>
-  <si>
-    <t>שחקן לז</t>
-  </si>
-  <si>
-    <t>שחקן לח</t>
-  </si>
-  <si>
-    <t>שחקן לט</t>
-  </si>
-  <si>
-    <t>שחקן מ</t>
-  </si>
-  <si>
-    <t>שחקן מא</t>
-  </si>
-  <si>
-    <t>שחקן מב</t>
-  </si>
-  <si>
-    <t>שחקן מג</t>
-  </si>
-  <si>
-    <t>שחקן מד</t>
-  </si>
-  <si>
-    <t>שחקן מה</t>
-  </si>
-  <si>
-    <t>שחקן מו</t>
-  </si>
-  <si>
-    <t>שחקן מז</t>
-  </si>
-  <si>
-    <t>שחקן מח</t>
-  </si>
-  <si>
-    <t>שחקן מט</t>
-  </si>
-  <si>
-    <t>שחקן נ</t>
-  </si>
-  <si>
-    <t>שחקן נא</t>
-  </si>
-  <si>
-    <t>שחקן נב</t>
+    <t>זיגי</t>
+  </si>
+  <si>
+    <t>טורצקי</t>
+  </si>
+  <si>
+    <t>גלי</t>
+  </si>
+  <si>
+    <t>הרצברג</t>
+  </si>
+  <si>
+    <t>עמרי נצן</t>
+  </si>
+  <si>
+    <t>שחר סלע</t>
+  </si>
+  <si>
+    <t>פייביש</t>
+  </si>
+  <si>
+    <t>דוידזון</t>
+  </si>
+  <si>
+    <t>יניב</t>
+  </si>
+  <si>
+    <t>מודן</t>
+  </si>
+  <si>
+    <t>בן שושן</t>
+  </si>
+  <si>
+    <t>זריהן</t>
+  </si>
+  <si>
+    <t>מנחה</t>
+  </si>
+  <si>
+    <t>שקד</t>
+  </si>
+  <si>
+    <t>סוירי</t>
+  </si>
+  <si>
+    <t>איילה</t>
+  </si>
+  <si>
+    <t>פינסלר</t>
+  </si>
+  <si>
+    <t>יובל בר</t>
+  </si>
+  <si>
+    <t>ירין</t>
+  </si>
+  <si>
+    <t>מיכאל</t>
+  </si>
+  <si>
+    <t>עדי טל</t>
+  </si>
+  <si>
+    <t>אורי ככ</t>
+  </si>
+  <si>
+    <t>שושני</t>
+  </si>
+  <si>
+    <t>אפרימה</t>
+  </si>
+  <si>
+    <t>אסף בן חיים</t>
+  </si>
+  <si>
+    <t>דור פרידמן</t>
+  </si>
+  <si>
+    <t>יזהר</t>
+  </si>
+  <si>
+    <t>ליעם מגיד</t>
+  </si>
+  <si>
+    <t>ליאם מור</t>
+  </si>
+  <si>
+    <t>נימי</t>
+  </si>
+  <si>
+    <t>גליקמן</t>
+  </si>
+  <si>
+    <t>עמית בר</t>
+  </si>
+  <si>
+    <t>עמית לוי</t>
+  </si>
+  <si>
+    <t>אליאב</t>
+  </si>
+  <si>
+    <t>אריאל בן אליעזר</t>
+  </si>
+  <si>
+    <t>דוד פיי</t>
+  </si>
+  <si>
+    <t>יהל שפי</t>
+  </si>
+  <si>
+    <t>יהלי מערבי ברנר</t>
+  </si>
+  <si>
+    <t>אברג'ל</t>
+  </si>
+  <si>
+    <t>נאמן</t>
+  </si>
+  <si>
+    <t>עידו קרן</t>
+  </si>
+  <si>
+    <t>תומר וקס</t>
+  </si>
+  <si>
+    <t>תומר קדם</t>
+  </si>
+  <si>
+    <t>אריאל ליבזון</t>
+  </si>
+  <si>
+    <t>גל ארצי</t>
+  </si>
+  <si>
+    <t>הילה</t>
+  </si>
+  <si>
+    <t>ליאורה</t>
+  </si>
+  <si>
+    <t>פסוול</t>
+  </si>
+  <si>
+    <t>מנקר</t>
+  </si>
+  <si>
+    <t>גרונר</t>
+  </si>
+  <si>
+    <t>תמיר</t>
+  </si>
+  <si>
+    <t>סטיב</t>
+  </si>
+  <si>
+    <t>גלעד חננאל</t>
+  </si>
+  <si>
+    <t>הוד</t>
+  </si>
+  <si>
+    <t>זהר רטנר</t>
+  </si>
+  <si>
+    <t>יואב סטרולוביץ'</t>
+  </si>
+  <si>
+    <t>עמרי קונסטנטינו</t>
+  </si>
+  <si>
+    <t>אביתר</t>
+  </si>
+  <si>
+    <t>ווינטרויב</t>
+  </si>
+  <si>
+    <t>גל נימצקי</t>
+  </si>
+  <si>
+    <t>דנה</t>
+  </si>
+  <si>
+    <t>יהל פורת</t>
+  </si>
+  <si>
+    <t>שליו</t>
+  </si>
+  <si>
+    <t>כהנא</t>
+  </si>
+  <si>
+    <t>רומנו</t>
   </si>
 </sst>
 </file>
@@ -467,8 +509,8 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -557,7 +599,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -572,7 +614,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -587,7 +629,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -602,7 +644,7 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -617,7 +659,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -632,7 +674,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -647,7 +689,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -662,7 +704,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -677,7 +719,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -692,7 +734,7 @@
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -707,7 +749,7 @@
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -722,7 +764,7 @@
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -737,7 +779,7 @@
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -752,7 +794,7 @@
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -767,7 +809,7 @@
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -782,7 +824,7 @@
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -797,7 +839,7 @@
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -812,7 +854,7 @@
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -827,7 +869,7 @@
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -842,7 +884,7 @@
       <c r="A25" s="2"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -857,7 +899,7 @@
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -872,7 +914,7 @@
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -887,7 +929,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
       <c r="C28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -902,7 +944,7 @@
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
       <c r="C29" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -917,7 +959,7 @@
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
       <c r="C30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1261,7 +1303,9 @@
     <row r="53" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -1274,7 +1318,9 @@
     <row r="54" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -1287,7 +1333,9 @@
     <row r="55" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -1300,7 +1348,9 @@
     <row r="56" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -1313,7 +1363,9 @@
     <row r="57" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -1326,7 +1378,9 @@
     <row r="58" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -1339,7 +1393,9 @@
     <row r="59" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -1352,7 +1408,9 @@
     <row r="60" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -1365,7 +1423,9 @@
     <row r="61" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -1378,7 +1438,9 @@
     <row r="62" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -1391,7 +1453,9 @@
     <row r="63" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -1404,7 +1468,9 @@
     <row r="64" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -1417,7 +1483,9 @@
     <row r="65" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="C65" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -1430,7 +1498,9 @@
     <row r="66" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="C66" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>

</xml_diff>